<commit_message>
Refined the code with possible error/logical error that may occur
</commit_message>
<xml_diff>
--- a/JPetStore-REF-Dispatcher/Data/Config.xlsx
+++ b/JPetStore-REF-Dispatcher/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/pratim_a_tarafder_capgemini_com/Documents/Documents/UiPath/JPetStore-REF-Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15D69274-445E-4F30-93F5-97A5A1FC4D98}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF7D7907-F735-479C-BFA0-33D2CDB773A5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -169,13 +169,31 @@
   </si>
   <si>
     <t>AssignmentFolder</t>
+  </si>
+  <si>
+    <t>Pet Category stores the Category of Pets</t>
+  </si>
+  <si>
+    <t>Category Fish</t>
+  </si>
+  <si>
+    <t>Category Cats</t>
+  </si>
+  <si>
+    <t>Category Reptiles</t>
+  </si>
+  <si>
+    <t>Category Birds</t>
+  </si>
+  <si>
+    <t>Category Dogs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -205,6 +223,11 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -226,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -237,6 +260,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,12 +585,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -614,7 +638,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -624,7 +648,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1643,12 +1667,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1685,7 +1709,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1696,7 +1720,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1810,7 +1834,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2802,16 +2826,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2864,11 +2888,76 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>